<commit_message>
The impact analysis is updated with the removed functionalities
</commit_message>
<xml_diff>
--- a/Monitor and Control/F_ImpactAnalysis.xlsx
+++ b/Monitor and Control/F_ImpactAnalysis.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d3db734411489fea/Desktop/Current QA/QA_Foodies/Monitor and Control/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8B681A-FEE0-43F0-A4DB-CFF754213223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{79C43B3D-F494-462A-9EA3-CD6B9C668935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2EA8191B-3803-4F18-969F-93D4F295DD5A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>The change</t>
   </si>
@@ -174,6 +174,45 @@
       </rPr>
       <t xml:space="preserve"> 1.0</t>
     </r>
+  </si>
+  <si>
+    <t>Add Admin' and 'Add User' are from the admin functionalities that the customer demanded.</t>
+  </si>
+  <si>
+    <t>Add Admin' and 'Add user' functionalities will be removed from all the system documents and middleware.</t>
+  </si>
+  <si>
+    <t>MEDIUM</t>
+  </si>
+  <si>
+    <t>The team members will be assigned on trello to remove the functionalities from the SRS, Use case, Sequence diagrams and disable it from the middleware.</t>
+  </si>
+  <si>
+    <t>The functionalities will be removed from the SRS, Use case, Sequence diagrams and diabled from the middleware.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time of testing will be reduced as the effort of testing of those functionalities is removed. </t>
+  </si>
+  <si>
+    <t>Search for restraunt' functionality will be removed from all the system documents and middleware.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add Admin' and 'Add User' functionalities is removed as per the customer's request. </t>
+  </si>
+  <si>
+    <t>Search for resdtraunt' functionality is asked by the project manager to be removed and the customer confirmed.</t>
+  </si>
+  <si>
+    <t>Search for restraunt' is from the user functionalities that the customer demanded.</t>
+  </si>
+  <si>
+    <t>The team members will be assigned on trello to remove this functionalitity from the SRS, Use case, Sequence diagrams and disable it from the middleware.</t>
+  </si>
+  <si>
+    <t>The functionality will be removed from the SRS, Use case, Sequence diagrams and diabled from the middleware.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time of testing will be reduced as the effort of testing of this functionalitity is removed. </t>
   </si>
 </sst>
 </file>
@@ -231,7 +270,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -254,11 +293,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -274,6 +337,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -622,8 +694,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{371CD6C8-DE74-48D7-B043-6CFFCE2F50A4}" name="Table3" displayName="Table3" ref="A1:G3" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A1:G3" xr:uid="{371CD6C8-DE74-48D7-B043-6CFFCE2F50A4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{371CD6C8-DE74-48D7-B043-6CFFCE2F50A4}" name="Table3" displayName="Table3" ref="A1:G5" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:G5" xr:uid="{371CD6C8-DE74-48D7-B043-6CFFCE2F50A4}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{898BBE53-B4CB-4985-9926-8F4E4EDE8303}" name="The change" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{69CF8660-9FDB-4EE0-A17F-49DC3729AA5F}" name="As-Is state" dataDxfId="5"/>
@@ -934,10 +1006,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA1E3C85-1AFD-4514-B244-55068F3EDA6B}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1021,18 +1093,64 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+    <row r="4" spans="1:7" ht="87.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="87.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>